<commit_message>
[Added] RF nuevos hasta el #16
</commit_message>
<xml_diff>
--- a/análisis/Requerimientos/Funcionales/RF05_Realizar check-in de la estadia del cliente..xlsx
+++ b/análisis/Requerimientos/Funcionales/RF05_Realizar check-in de la estadia del cliente..xlsx
@@ -263,23 +263,23 @@
     <t>RF05</t>
   </si>
   <si>
-    <t>Realizar check-in de la estadia del cliente.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El sistema debe realizar un check-in cuando un cliente se registre y salga del Hostal. </t>
-  </si>
-  <si>
-    <t>El sistema debe realizar un check-in cuando un cliente se registre y salga del Hostal. Además de almacenar el nombre,rut, dirección, metodo de pago del cliente, además de si necesita alguna dieta especial, o tiene alguna enfermedad o alergia que afecte su estadia en la Hostal.</t>
-  </si>
-  <si>
     <t>Alta</t>
+  </si>
+  <si>
+    <t>Realizar check-in y check-out de la estadia del cliente.</t>
+  </si>
+  <si>
+    <t>El sistema debe realizar un check-in cuando un cliente se registre y un check-out cuando salga del Hostal. Además de almacenar el nombre,rut, dirección, metodo de pago del cliente, además de si necesita alguna dieta especial, o tiene alguna enfermedad o alergia que afecte su estadia en la Hostal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe realizar un check-in cuando un cliente se registre y un check-out cuando salga del Hostal. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +319,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -457,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -484,6 +492,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E13"/>
+  <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +788,7 @@
     <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,23 +796,23 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -813,17 +822,17 @@
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
@@ -833,27 +842,27 @@
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
@@ -862,8 +871,9 @@
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
@@ -871,7 +881,7 @@
       <c r="D12" s="9"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -889,7 +899,7 @@
     <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>